<commit_message>
changed clutter change variables
</commit_message>
<xml_diff>
--- a/clutter_change_order_cb.xlsx
+++ b/clutter_change_order_cb.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backups\All Files\Genel\Is\2022\Upwork\LabX\studies\materials\drivingSimulator\repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659BBFE3-8BFA-4E73-9316-1C0D5D261BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8199C540-1F7F-4E2B-9709-16FB3A49F6F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -388,8 +388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="K69" sqref="K69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,7 +504,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -668,7 +668,7 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -686,7 +686,7 @@
         <v>12</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -839,7 +839,7 @@
         <v>0</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19" s="1"/>
     </row>
@@ -887,7 +887,7 @@
         <v>0</v>
       </c>
       <c r="G21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21" s="1"/>
     </row>
@@ -1124,7 +1124,7 @@
         <v>0</v>
       </c>
       <c r="F31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G31">
         <v>1</v>
@@ -1169,7 +1169,7 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -1468,7 +1468,7 @@
         <v>21</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -1546,7 +1546,7 @@
         <v>0</v>
       </c>
       <c r="G49">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1609,7 +1609,7 @@
         <v>0</v>
       </c>
       <c r="E52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F52">
         <v>0</v>
@@ -1997,7 +1997,7 @@
         <v>20</v>
       </c>
       <c r="D69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E69">
         <v>0</v>
@@ -2049,7 +2049,7 @@
         <v>1</v>
       </c>
       <c r="F71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G71">
         <v>0</v>
@@ -2075,7 +2075,7 @@
         <v>0</v>
       </c>
       <c r="G72">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>